<commit_message>
Add xml to sql server
</commit_message>
<xml_diff>
--- a/Excel/Computers.xlsx
+++ b/Excel/Computers.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,19 +30,19 @@
     <t>ProcessorId</t>
   </si>
   <si>
-    <t>MemoryId</t>
-  </si>
-  <si>
     <t>VideocardId</t>
   </si>
   <si>
     <t>Price</t>
   </si>
+  <si>
+    <t>MemorycardId</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,7 +352,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -363,14 +363,14 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="A1:G8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -385,13 +385,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added new items to the excel files
</commit_message>
<xml_diff>
--- a/Excel/Computers.xlsx
+++ b/Excel/Computers.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,7 +352,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,6 +494,506 @@
         <v>500</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>13</v>
+      </c>
+      <c r="F12">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>9</v>
+      </c>
+      <c r="F18">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>6</v>
+      </c>
+      <c r="F30">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <v>600</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel file names changed to follow convention
Some of the Excel file names were changed to follow the names of corresponding model types, i.e. Memories.xlsx changed to Memorycards.xlsx;
One record in Computers with changed VideocardId to "1" due to missing vidiocard with Id "13";
In Merorycards.xlsx some strange properties (F3, F4..) were erroneously detected by the parser, so this file was re-created with the same data.
</commit_message>
<xml_diff>
--- a/Excel/Computers.xlsx
+++ b/Excel/Computers.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -363,7 +363,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +608,7 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>1400</v>

</xml_diff>